<commit_message>
Johnson problem import bug fix
</commit_message>
<xml_diff>
--- a/AdditionalFiles/test.xlsx
+++ b/AdditionalFiles/test.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
   <si>
     <t>Тест1</t>
   </si>
@@ -103,12 +103,24 @@
   </si>
   <si>
     <t>работа3</t>
+  </si>
+  <si>
+    <t>Процессы:</t>
+  </si>
+  <si>
+    <t>исполнитель</t>
+  </si>
+  <si>
+    <t>работа</t>
+  </si>
+  <si>
+    <t>время</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,12 +171,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,18 +460,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D9:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
@@ -468,7 +482,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
         <v>0</v>
       </c>
@@ -482,7 +496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>2</v>
       </c>
@@ -508,7 +522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>4</v>
       </c>
@@ -525,7 +539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -551,12 +565,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>6</v>
       </c>
@@ -566,8 +583,20 @@
       <c r="G15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>7</v>
       </c>
@@ -577,8 +606,20 @@
       <c r="G16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>8</v>
       </c>
@@ -588,16 +629,34 @@
       <c r="G17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17">
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <v>22</v>
+      </c>
+      <c r="N17">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>2</v>
       </c>
@@ -610,8 +669,20 @@
       <c r="H19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>4</v>
       </c>
@@ -624,8 +695,11 @@
       <c r="H20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>14</v>
       </c>
@@ -638,13 +712,28 @@
       <c r="H21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E22" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>6</v>
       </c>
@@ -654,8 +743,20 @@
       <c r="G23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>7</v>
       </c>
@@ -665,8 +766,20 @@
       <c r="G24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>8</v>
       </c>
@@ -676,8 +789,20 @@
       <c r="G25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25">
+        <v>13</v>
+      </c>
+      <c r="M25">
+        <v>22</v>
+      </c>
+      <c r="N25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>13</v>
       </c>
@@ -685,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>2</v>
       </c>
@@ -699,7 +824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>4</v>
       </c>
@@ -713,7 +838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>14</v>
       </c>
@@ -727,12 +852,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E30" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
         <v>6</v>
       </c>
@@ -743,7 +868,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
         <v>7</v>
       </c>
@@ -754,7 +879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>8</v>
       </c>

</xml_diff>